<commit_message>
Whole Test Cases Run
</commit_message>
<xml_diff>
--- a/ERP_Hybrid/FileInput/Controller.xlsx
+++ b/ERP_Hybrid/FileInput/Controller.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation_Testing\ERP_Hybrid\FileInput\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uccha\git\Hybrid-With-Maven-\ERP_Hybrid\FileInput\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{122CC84C-B398-4C7C-BDF9-CF30345F7CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA5E64C-6DCE-4A97-BEDC-2429F698566C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{34A0AAA5-6E4B-4BFA-B178-9673BA870147}"/>
   </bookViews>
@@ -941,7 +941,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1023,7 +1023,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1244,8 +1244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59CEE043-DB44-4773-A6EB-DC2513D676B1}">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>